<commit_message>
Enhance validation process by adding typo detection for input data against field options. Introduce functions for loading field options and calculating Levenshtein distance for suggesting close matches. Update field options in JSON files for consistency.
</commit_message>
<xml_diff>
--- a/input_tables/blueprint_tasks.xlsx
+++ b/input_tables/blueprint_tasks.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="55">
   <si>
     <t>task</t>
   </si>
@@ -37,7 +37,7 @@
     <t>Blur</t>
   </si>
   <si>
-    <t>client, IM_operators, auto</t>
+    <t>client, IM-operators, auto</t>
   </si>
   <si>
     <t>Photo enhancement</t>
@@ -46,7 +46,7 @@
     <t>Photo-enhancement</t>
   </si>
   <si>
-    <t>IM_operators, auto</t>
+    <t>IM-operators, auto</t>
   </si>
   <si>
     <t>HDR Photos</t>
@@ -58,7 +58,7 @@
     <t/>
   </si>
   <si>
-    <t>IM_operators</t>
+    <t>IM-operators</t>
   </si>
   <si>
     <t>Auto HDR Photos</t>
@@ -94,7 +94,7 @@
     <t>Panos, geometry-scaffold</t>
   </si>
   <si>
-    <t>client, auto, IM_operators</t>
+    <t>client, auto, IM-operators</t>
   </si>
   <si>
     <t>Pano Generation</t>
@@ -122,9 +122,6 @@
   </si>
   <si>
     <t>geometry-scaffold</t>
-  </si>
-  <si>
-    <t>IM-operators</t>
   </si>
   <si>
     <t>floorplan-building</t>
@@ -885,18 +882,18 @@
         <v>14</v>
       </c>
       <c r="E19" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" t="s">
         <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D20" t="s">
         <v>14</v>
@@ -907,13 +904,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" t="s">
         <v>36</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D21" t="s">
         <v>14</v>
@@ -924,13 +921,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22" t="s">
         <v>36</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D22" t="s">
         <v>14</v>
@@ -941,13 +938,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B23" t="s">
         <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D23" t="s">
         <v>14</v>
@@ -958,13 +955,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" t="s">
         <v>46</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>47</v>
-      </c>
-      <c r="C24" t="s">
-        <v>48</v>
       </c>
       <c r="D24" t="s">
         <v>14</v>
@@ -975,13 +972,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" t="s">
         <v>49</v>
-      </c>
-      <c r="B25" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" t="s">
-        <v>50</v>
       </c>
       <c r="D25" t="s">
         <v>14</v>
@@ -992,13 +989,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" t="s">
         <v>51</v>
-      </c>
-      <c r="B26" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" t="s">
-        <v>52</v>
       </c>
       <c r="D26" t="s">
         <v>14</v>
@@ -1009,13 +1006,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" t="s">
         <v>53</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>54</v>
-      </c>
-      <c r="C27" t="s">
-        <v>55</v>
       </c>
       <c r="D27" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Enhance available_options.json with task responsibilities, producers, and enhancements; remove deprecated field_options.json. Update validation logic to utilize new mappings for improved data integrity and management.
</commit_message>
<xml_diff>
--- a/input_tables/blueprint_tasks.xlsx
+++ b/input_tables/blueprint_tasks.xlsx
@@ -95,7 +95,7 @@
     <t xml:space="preserve">Geometry-building-roomPlan</t>
   </si>
   <si>
-    <t xml:space="preserve">Roomplan-FP</t>
+    <t xml:space="preserve">roomplan-FP</t>
   </si>
   <si>
     <t xml:space="preserve">Geometry-building-precon</t>
@@ -176,7 +176,7 @@
     <t xml:space="preserve">Walkthrough-video-generation</t>
   </si>
   <si>
-    <t xml:space="preserve">Walkthrough video</t>
+    <t xml:space="preserve">Walkthrough-video</t>
   </si>
   <si>
     <t xml:space="preserve">Photo-Capture</t>
@@ -356,8 +356,8 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Enhance available_options.json with new task responsibilities, producers, and enhancements. Update transformation functions to build relationships between tasks and task products during processing. Refactor relationship building logic for improved data management and accuracy.
</commit_message>
<xml_diff>
--- a/input_tables/blueprint_tasks.xlsx
+++ b/input_tables/blueprint_tasks.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="65">
   <si>
     <t xml:space="preserve">task</t>
   </si>
@@ -89,21 +89,27 @@
     <t xml:space="preserve">geometry-scaffold</t>
   </si>
   <si>
+    <t xml:space="preserve">IM-operators, auto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geometry-building-roomPlan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">roomplan-FP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IM-operators, client</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geometry-building-precon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preconInput</t>
+  </si>
+  <si>
     <t xml:space="preserve">IM-operators</t>
   </si>
   <si>
-    <t xml:space="preserve">Geometry-building-roomPlan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">roomplan-FP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geometry-building-precon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preconInput</t>
-  </si>
-  <si>
     <t xml:space="preserve">floorplan-building</t>
   </si>
   <si>
@@ -207,9 +213,6 @@
   </si>
   <si>
     <t xml:space="preserve">Photo-enhancement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IM-operators, auto</t>
   </si>
   <si>
     <t xml:space="preserve">HDR-Photo-enhancement</t>
@@ -356,8 +359,8 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -449,33 +452,33 @@
         <v>15</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>11</v>
@@ -483,13 +486,13 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>11</v>
@@ -497,13 +500,13 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>11</v>
@@ -511,13 +514,13 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>11</v>
@@ -525,13 +528,13 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E15" s="0" t="s">
         <v>11</v>
@@ -540,13 +543,13 @@
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>11</v>
@@ -554,13 +557,13 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E18" s="0" t="s">
         <v>11</v>
@@ -568,13 +571,13 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>11</v>
@@ -582,27 +585,27 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E21" s="0" t="s">
         <v>11</v>
@@ -610,13 +613,13 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="0" t="s">
-        <v>42</v>
-      </c>
       <c r="C22" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>11</v>
@@ -625,16 +628,16 @@
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -643,7 +646,7 @@
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>10</v>
@@ -652,32 +655,32 @@
         <v>10</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="B30" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>51</v>
-      </c>
       <c r="E30" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>10</v>
@@ -686,32 +689,32 @@
         <v>10</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="B32" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>55</v>
-      </c>
       <c r="E32" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>10</v>
@@ -720,32 +723,32 @@
         <v>10</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="B34" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>59</v>
-      </c>
       <c r="E34" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>10</v>
@@ -754,27 +757,27 @@
         <v>10</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="B36" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>62</v>
-      </c>
       <c r="E36" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>